<commit_message>
agregado FA Latam - faltan puntuales de FA y EE.
</commit_message>
<xml_diff>
--- a/input.xlsx
+++ b/input.xlsx
@@ -28,14 +28,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="50">
   <si>
     <t>showFeed</t>
   </si>
   <si>
-    <t>showName</t>
-  </si>
-  <si>
     <t>genDateStr</t>
   </si>
   <si>
@@ -100,9 +97,6 @@
   </si>
   <si>
     <t>OFFAIR</t>
-  </si>
-  <si>
-    <t>lala land</t>
   </si>
   <si>
     <t>la la land usa</t>
@@ -211,13 +205,7 @@
     </r>
   </si>
   <si>
-    <t>Los fogones tradicionales. Argentina</t>
-  </si>
-  <si>
     <t>CAPS ESTRENO</t>
-  </si>
-  <si>
-    <t>Los fogones tradicionales. México</t>
   </si>
   <si>
     <t>BUMP</t>
@@ -244,12 +232,39 @@
   <si>
     <t>MARATON</t>
   </si>
+  <si>
+    <t>Breaking music</t>
+  </si>
+  <si>
+    <t>dowton abbey</t>
+  </si>
+  <si>
+    <t>padre brown</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">showName
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Cuerpo)"/>
+      </rPr>
+      <t>Usar la validacion para dejar indicaciones al usuario</t>
+    </r>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -320,6 +335,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri (Cuerpo)"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -368,7 +389,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -393,6 +414,9 @@
     <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -676,7 +700,7 @@
   <dimension ref="A1:N50"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -701,44 +725,44 @@
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="E1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="F1" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="G1" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="H1" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="I1" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="J1" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="E1" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="G1" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="H1" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="I1" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="J1" s="11" t="s">
-        <v>4</v>
-      </c>
       <c r="K1" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="L1" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="L1" s="11" t="s">
+      <c r="M1" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="M1" s="11" t="s">
+      <c r="N1" s="11" t="s">
         <v>8</v>
-      </c>
-      <c r="N1" s="11" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
@@ -746,16 +770,16 @@
         <v>11</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>44</v>
+        <v>27</v>
       </c>
       <c r="D2" s="15">
-        <v>44105.75</v>
+        <v>44129.916666666664</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>26</v>
+        <v>49</v>
       </c>
       <c r="F2" s="16">
         <v>44105</v>
@@ -764,42 +788,42 @@
         <v>44135</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J2" s="6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="K2" s="6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="L2" s="6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="M2" s="6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="N2" s="6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="D3" s="15">
-        <v>44105.625</v>
+        <v>44129.916666666664</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>27</v>
+        <v>49</v>
       </c>
       <c r="F3" s="16">
         <v>44105</v>
@@ -808,25 +832,25 @@
         <v>44135</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I3" s="6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J3" s="6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="K3" s="6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="L3" s="6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="M3" s="6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="N3" s="6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
@@ -834,16 +858,16 @@
         <v>11</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>46</v>
+        <v>30</v>
       </c>
       <c r="D4" s="15">
         <v>43922.916666666664</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F4" s="16">
         <v>44109</v>
@@ -852,42 +876,42 @@
         <v>44135</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I4" s="6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J4" s="6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K4" s="6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="L4" s="6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="M4" s="6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="N4" s="6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>24</v>
+        <v>47</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>46</v>
+        <v>28</v>
       </c>
       <c r="D5" s="15">
         <v>44109.625</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F5" s="16">
         <v>44136</v>
@@ -896,42 +920,42 @@
         <v>44135</v>
       </c>
       <c r="H5" s="6" t="s">
-        <v>5</v>
+        <v>35</v>
       </c>
       <c r="I5" s="6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J5" s="6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="K5" s="6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="L5" s="6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="M5" s="6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="N5" s="6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>46</v>
+        <v>27</v>
       </c>
       <c r="D6" s="15">
         <v>44110.583333333336</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F6" s="16">
         <v>44168</v>
@@ -940,25 +964,25 @@
         <v>44135</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I6" s="6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J6" s="6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="K6" s="6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="L6" s="6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="M6" s="6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="N6" s="6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
@@ -1709,26 +1733,26 @@
     <col min="2" max="2" width="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B2" s="19" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
@@ -1737,15 +1761,15 @@
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
@@ -1754,97 +1778,97 @@
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B4" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4" s="6"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" s="6"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" s="6"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="C4" s="6"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A5" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="B5" s="8" t="s">
+      <c r="C7" s="6"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="C5" s="6"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A6" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6" s="8" t="s">
+      <c r="C8" s="6"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" s="6"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="C6" s="6"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A7" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="B7" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="C7" s="6"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A8" s="7" t="s">
+      <c r="C10" s="6"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" s="6"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A12" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="C8" s="6"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A9" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="C9" s="6"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A10" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="B10" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="C10" s="6"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A11" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B11" s="17" t="s">
-        <v>35</v>
-      </c>
-      <c r="C11" s="6"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A12" s="7" t="s">
+      <c r="B12" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="C12" s="6"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A13" s="7" t="s">
         <v>14</v>
-      </c>
-      <c r="B12" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="C12" s="6"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A13" s="7" t="s">
-        <v>15</v>
       </c>
       <c r="B13" s="9"/>
       <c r="C13" s="6"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B14" s="9"/>
       <c r="C14" s="6"/>

</xml_diff>

<commit_message>
agregado algunas de AMC y puntuales FA y EE.
</commit_message>
<xml_diff>
--- a/input.xlsx
+++ b/input.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="80" yWindow="460" windowWidth="23860" windowHeight="10140" tabRatio="500"/>
+    <workbookView xWindow="80" yWindow="460" windowWidth="23860" windowHeight="10140" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="55">
   <si>
     <t>showFeed</t>
   </si>
@@ -42,9 +42,6 @@
     <t>crossChannel</t>
   </si>
   <si>
-    <t>True</t>
-  </si>
-  <si>
     <t>megaCable</t>
   </si>
   <si>
@@ -93,15 +90,9 @@
     <t>FABRASIL</t>
   </si>
   <si>
-    <t>AMCNETWORKS</t>
-  </si>
-  <si>
     <t>OFFAIR</t>
   </si>
   <si>
-    <t>la la land usa</t>
-  </si>
-  <si>
     <t>lunes a viernes</t>
   </si>
   <si>
@@ -135,42 +126,7 @@
     <t>MEDIODIA</t>
   </si>
   <si>
-    <t>False</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">dstMex
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>True si MEX adelanta la hora, False si no.</t>
-    </r>
-  </si>
-  <si>
     <t>Booleans</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">dstChi
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>True si Chile adelanta la hora, False si no.</t>
-    </r>
   </si>
   <si>
     <r>
@@ -233,15 +189,6 @@
     <t>MARATON</t>
   </si>
   <si>
-    <t>Breaking music</t>
-  </si>
-  <si>
-    <t>dowton abbey</t>
-  </si>
-  <si>
-    <t>padre brown</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">showName
 </t>
@@ -257,7 +204,75 @@
     </r>
   </si>
   <si>
-    <t>no</t>
+    <t>Breaking music 2</t>
+  </si>
+  <si>
+    <t>NO</t>
+  </si>
+  <si>
+    <t>PIPIRIPI</t>
+  </si>
+  <si>
+    <t>padre brown 4</t>
+  </si>
+  <si>
+    <t>dowton abbey 6</t>
+  </si>
+  <si>
+    <t>foxtrot 3</t>
+  </si>
+  <si>
+    <t>maxsuanba 5</t>
+  </si>
+  <si>
+    <t>EPISODICAS</t>
+  </si>
+  <si>
+    <t>Promo Mediodia se vende como GEN</t>
+  </si>
+  <si>
+    <t>SI</t>
+  </si>
+  <si>
+    <t>chicas poderosas</t>
+  </si>
+  <si>
+    <t>miercoles 7 a domingo 12</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">dstMex
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>MEX adelanta la hora?</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">dstChi
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Chile adelanta la hora?</t>
+    </r>
+  </si>
+  <si>
+    <t>_AMCNETWORKS</t>
   </si>
 </sst>
 </file>
@@ -697,10 +712,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N50"/>
+  <dimension ref="A1:N53"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -709,7 +724,7 @@
     <col min="2" max="2" width="41.6640625" customWidth="1"/>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="27.83203125" customWidth="1"/>
-    <col min="5" max="5" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.6640625" customWidth="1"/>
     <col min="6" max="6" width="15.1640625" customWidth="1"/>
     <col min="7" max="7" width="15" customWidth="1"/>
     <col min="8" max="8" width="12.33203125" customWidth="1"/>
@@ -726,328 +741,440 @@
         <v>0</v>
       </c>
       <c r="B1" s="20" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="C1" s="11" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="E1" s="11" t="s">
         <v>1</v>
       </c>
       <c r="F1" s="13" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="G1" s="13" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="H1" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="I1" s="13" t="s">
-        <v>38</v>
+        <v>52</v>
+      </c>
+      <c r="I1" s="20" t="s">
+        <v>53</v>
       </c>
       <c r="J1" s="11" t="s">
         <v>3</v>
       </c>
       <c r="K1" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="L1" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="L1" s="11" t="s">
+      <c r="M1" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="M1" s="11" t="s">
+      <c r="N1" s="11" t="s">
         <v>7</v>
-      </c>
-      <c r="N1" s="11" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="D2" s="15">
-        <v>44129.916666666664</v>
+        <v>44111.916666666664</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="F2" s="16">
         <v>44105</v>
       </c>
       <c r="G2" s="16">
-        <v>44135</v>
+        <v>44116</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>4</v>
+        <v>49</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>4</v>
+        <v>49</v>
       </c>
       <c r="J2" s="6" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="K2" s="6" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="L2" s="6" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="M2" s="6" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="N2" s="6" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="D3" s="15">
-        <v>44129.916666666664</v>
+        <v>44111.916666666664</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="F3" s="16">
         <v>44105</v>
       </c>
       <c r="G3" s="16">
-        <v>44135</v>
+        <v>44116</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>4</v>
+        <v>49</v>
       </c>
       <c r="I3" s="6" t="s">
-        <v>4</v>
+        <v>49</v>
       </c>
       <c r="J3" s="6" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="K3" s="6" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="L3" s="6" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="M3" s="6" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="N3" s="6" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="C4" s="14" t="s">
         <v>30</v>
       </c>
       <c r="D4" s="15">
-        <v>43922.916666666664</v>
+        <v>44111.916666666664</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>26</v>
+        <v>51</v>
       </c>
       <c r="F4" s="16">
-        <v>44109</v>
+        <v>44105</v>
       </c>
       <c r="G4" s="16">
-        <v>44135</v>
+        <v>44116</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>4</v>
+        <v>49</v>
       </c>
       <c r="I4" s="6" t="s">
-        <v>4</v>
+        <v>49</v>
       </c>
       <c r="J4" s="6" t="s">
-        <v>4</v>
+        <v>41</v>
       </c>
       <c r="K4" s="6" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="L4" s="6" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="M4" s="6" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="N4" s="6" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D5" s="15">
-        <v>44109.625</v>
+        <v>44111.916666666664</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>24</v>
+        <v>51</v>
       </c>
       <c r="F5" s="16">
-        <v>44136</v>
+        <v>44105</v>
       </c>
       <c r="G5" s="16">
-        <v>44135</v>
+        <v>44116</v>
       </c>
       <c r="H5" s="6" t="s">
-        <v>35</v>
+        <v>49</v>
       </c>
       <c r="I5" s="6" t="s">
-        <v>4</v>
+        <v>49</v>
       </c>
       <c r="J5" s="6" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="K5" s="6" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="L5" s="6" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="M5" s="6" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="N5" s="6" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>23</v>
+        <v>40</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D6" s="15">
-        <v>44110.583333333336</v>
+        <v>44129.916666666664</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>25</v>
+        <v>42</v>
       </c>
       <c r="F6" s="16">
-        <v>44168</v>
+        <v>44105</v>
       </c>
       <c r="G6" s="16">
         <v>44135</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>4</v>
+        <v>49</v>
       </c>
       <c r="I6" s="6" t="s">
-        <v>4</v>
+        <v>49</v>
       </c>
       <c r="J6" s="6" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="K6" s="6" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="L6" s="6" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="M6" s="6" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="N6" s="6" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A7" s="6"/>
-      <c r="B7" s="6"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="6"/>
-      <c r="I7" s="6"/>
-      <c r="J7" s="6"/>
-      <c r="K7" s="6"/>
-      <c r="L7" s="6"/>
-      <c r="M7" s="6"/>
-      <c r="N7" s="6"/>
+      <c r="A7" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" s="15">
+        <v>43922.916666666664</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F7" s="16">
+        <v>44109</v>
+      </c>
+      <c r="G7" s="16">
+        <v>44135</v>
+      </c>
+      <c r="H7" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="I7" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="J7" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="K7" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="L7" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="M7" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="N7" s="6" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A8" s="6"/>
-      <c r="B8" s="6"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6"/>
-      <c r="H8" s="6"/>
-      <c r="I8" s="6"/>
-      <c r="J8" s="6"/>
-      <c r="K8" s="6"/>
-      <c r="L8" s="6"/>
-      <c r="M8" s="6"/>
-      <c r="N8" s="6"/>
+      <c r="A8" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="D8" s="15">
+        <v>44109.625</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="F8" s="16">
+        <v>44136</v>
+      </c>
+      <c r="G8" s="16">
+        <v>44135</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="I8" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="J8" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="K8" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="L8" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="M8" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="N8" s="6" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A9" s="6"/>
-      <c r="B9" s="6"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6"/>
-      <c r="H9" s="6"/>
-      <c r="I9" s="6"/>
-      <c r="J9" s="6"/>
-      <c r="K9" s="6"/>
-      <c r="L9" s="6"/>
-      <c r="M9" s="6"/>
-      <c r="N9" s="6"/>
+      <c r="A9" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" s="15">
+        <v>44110.583333333336</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="F9" s="16">
+        <v>44168</v>
+      </c>
+      <c r="G9" s="16">
+        <v>44135</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="I9" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="J9" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="K9" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="L9" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="M9" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="N9" s="6" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A10" s="6"/>
-      <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
-      <c r="I10" s="6"/>
-      <c r="J10" s="6"/>
-      <c r="K10" s="6"/>
-      <c r="L10" s="6"/>
-      <c r="M10" s="6"/>
-      <c r="N10" s="6"/>
+      <c r="A10" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="C10" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="D10" s="15">
+        <v>43922.916666666664</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F10" s="16">
+        <v>44109</v>
+      </c>
+      <c r="G10" s="16">
+        <v>44135</v>
+      </c>
+      <c r="H10" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="I10" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="J10" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="K10" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="L10" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="M10" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="N10" s="6" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" s="6"/>
@@ -1689,6 +1816,54 @@
       <c r="M50" s="6"/>
       <c r="N50" s="6"/>
     </row>
+    <row r="51" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A51" s="6"/>
+      <c r="B51" s="6"/>
+      <c r="C51" s="6"/>
+      <c r="D51" s="6"/>
+      <c r="E51" s="6"/>
+      <c r="F51" s="6"/>
+      <c r="G51" s="6"/>
+      <c r="H51" s="6"/>
+      <c r="I51" s="6"/>
+      <c r="J51" s="6"/>
+      <c r="K51" s="6"/>
+      <c r="L51" s="6"/>
+      <c r="M51" s="6"/>
+      <c r="N51" s="6"/>
+    </row>
+    <row r="52" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A52" s="6"/>
+      <c r="B52" s="6"/>
+      <c r="C52" s="6"/>
+      <c r="D52" s="6"/>
+      <c r="E52" s="6"/>
+      <c r="F52" s="6"/>
+      <c r="G52" s="6"/>
+      <c r="H52" s="6"/>
+      <c r="I52" s="6"/>
+      <c r="J52" s="6"/>
+      <c r="K52" s="6"/>
+      <c r="L52" s="6"/>
+      <c r="M52" s="6"/>
+      <c r="N52" s="6"/>
+    </row>
+    <row r="53" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A53" s="6"/>
+      <c r="B53" s="6"/>
+      <c r="C53" s="6"/>
+      <c r="D53" s="6"/>
+      <c r="E53" s="6"/>
+      <c r="F53" s="6"/>
+      <c r="G53" s="6"/>
+      <c r="H53" s="6"/>
+      <c r="I53" s="6"/>
+      <c r="J53" s="6"/>
+      <c r="K53" s="6"/>
+      <c r="L53" s="6"/>
+      <c r="M53" s="6"/>
+      <c r="N53" s="6"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1699,19 +1874,19 @@
           <x14:formula1>
             <xm:f>Validacion!$A$2:$A$14</xm:f>
           </x14:formula1>
-          <xm:sqref>A2:A42</xm:sqref>
+          <xm:sqref>A2:A45</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Validacion!$B$2:$B$14</xm:f>
           </x14:formula1>
-          <xm:sqref>C2:C43</xm:sqref>
+          <xm:sqref>C2:C46</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Validacion!$C$2:$C$3</xm:f>
           </x14:formula1>
-          <xm:sqref>H2:N50</xm:sqref>
+          <xm:sqref>H2:N53</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1723,8 +1898,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1735,24 +1910,24 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>2</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
-        <v>19</v>
+        <v>54</v>
       </c>
       <c r="B2" s="19" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
@@ -1766,10 +1941,10 @@
         <v>18</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>4</v>
+        <v>49</v>
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
@@ -1780,95 +1955,100 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C4" s="6"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C5" s="6"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C6" s="6"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B7" s="17" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C7" s="6"/>
+      <c r="D7" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C8" s="6"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C9" s="6"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C10" s="6"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B11" s="17" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C11" s="6"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B12" s="18" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="C12" s="6"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="B13" s="9"/>
+        <v>13</v>
+      </c>
+      <c r="B13" s="18" t="s">
+        <v>47</v>
+      </c>
       <c r="C13" s="6"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="7" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B14" s="9"/>
       <c r="C14" s="6"/>
@@ -1887,8 +2067,8 @@
       <c r="C22" s="3"/>
     </row>
   </sheetData>
-  <sortState ref="B2:B11">
-    <sortCondition ref="B2"/>
+  <sortState ref="A2:A14">
+    <sortCondition ref="A2"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
promos GEN_SERIES. Allowed days. horarios 1 digito
</commit_message>
<xml_diff>
--- a/input.xlsx
+++ b/input.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="80" yWindow="460" windowWidth="23860" windowHeight="10140" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="80" yWindow="460" windowWidth="23860" windowHeight="10140" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="50">
   <si>
     <t>showFeed</t>
   </si>
@@ -93,15 +93,6 @@
     <t>OFFAIR</t>
   </si>
   <si>
-    <t>lunes a viernes</t>
-  </si>
-  <si>
-    <t>martes y jueves</t>
-  </si>
-  <si>
-    <t>miercoles</t>
-  </si>
-  <si>
     <t>ESTRENO</t>
   </si>
   <si>
@@ -121,9 +112,6 @@
   </si>
   <si>
     <t>STUNT</t>
-  </si>
-  <si>
-    <t>MEDIODIA</t>
   </si>
   <si>
     <t>Booleans</t>
@@ -186,9 +174,6 @@
     </r>
   </si>
   <si>
-    <t>MARATON</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">showName
 </t>
@@ -204,27 +189,9 @@
     </r>
   </si>
   <si>
-    <t>Breaking music 2</t>
-  </si>
-  <si>
     <t>NO</t>
   </si>
   <si>
-    <t>PIPIRIPI</t>
-  </si>
-  <si>
-    <t>padre brown 4</t>
-  </si>
-  <si>
-    <t>dowton abbey 6</t>
-  </si>
-  <si>
-    <t>foxtrot 3</t>
-  </si>
-  <si>
-    <t>maxsuanba 5</t>
-  </si>
-  <si>
     <t>EPISODICAS</t>
   </si>
   <si>
@@ -232,12 +199,6 @@
   </si>
   <si>
     <t>SI</t>
-  </si>
-  <si>
-    <t>chicas poderosas</t>
-  </si>
-  <si>
-    <t>miercoles 7 a domingo 12</t>
   </si>
   <si>
     <r>
@@ -273,6 +234,30 @@
   </si>
   <si>
     <t>_AMCNETWORKS</t>
+  </si>
+  <si>
+    <t>Promo Maraton se vende como Puntual</t>
+  </si>
+  <si>
+    <t>GEN_SERIES</t>
+  </si>
+  <si>
+    <t>GEN_SERIES es para las promos genéricas de series de AMC</t>
+  </si>
+  <si>
+    <t>lunes</t>
+  </si>
+  <si>
+    <t>BOTTOMLESS BRUNCH AT COLEMAN TEMP 2</t>
+  </si>
+  <si>
+    <t>FEAR THE WALKING DEAD S6A</t>
+  </si>
+  <si>
+    <t>GUARDIANES DE TRADICION</t>
+  </si>
+  <si>
+    <t>MARTES</t>
   </si>
 </sst>
 </file>
@@ -404,7 +389,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -426,7 +411,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -714,8 +698,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N53"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -740,29 +724,29 @@
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="20" t="s">
-        <v>39</v>
+      <c r="B1" s="19" t="s">
+        <v>34</v>
       </c>
       <c r="C1" s="11" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="E1" s="11" t="s">
         <v>1</v>
       </c>
       <c r="F1" s="13" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="G1" s="13" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="H1" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="I1" s="20" t="s">
-        <v>53</v>
+        <v>39</v>
+      </c>
+      <c r="I1" s="19" t="s">
+        <v>40</v>
       </c>
       <c r="J1" s="11" t="s">
         <v>3</v>
@@ -785,43 +769,43 @@
         <v>18</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="D2" s="15">
-        <v>44111.916666666664</v>
+        <v>44109.916666666664</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="F2" s="16">
-        <v>44105</v>
+        <v>44080</v>
       </c>
       <c r="G2" s="16">
-        <v>44116</v>
+        <v>44104</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="J2" s="6" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="K2" s="6" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="L2" s="6" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="M2" s="6" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="N2" s="6" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
@@ -829,43 +813,43 @@
         <v>17</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="D3" s="15">
-        <v>44111.916666666664</v>
+        <v>44109.916666666664</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="F3" s="16">
-        <v>44105</v>
+        <v>44080</v>
       </c>
       <c r="G3" s="16">
-        <v>44116</v>
+        <v>44104</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="I3" s="6" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="J3" s="6" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="K3" s="6" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="L3" s="6" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="M3" s="6" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="N3" s="6" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
@@ -873,43 +857,43 @@
         <v>16</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="D4" s="15">
-        <v>44111.916666666664</v>
+        <v>44109.916666666664</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="F4" s="16">
-        <v>44105</v>
+        <v>44080</v>
       </c>
       <c r="G4" s="16">
-        <v>44116</v>
+        <v>44104</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="I4" s="6" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="J4" s="6" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="K4" s="6" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="L4" s="6" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="M4" s="6" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="N4" s="6" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
@@ -917,263 +901,263 @@
         <v>15</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="D5" s="15">
-        <v>44111.916666666664</v>
+        <v>44109.916666666664</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="F5" s="16">
-        <v>44105</v>
+        <v>44080</v>
       </c>
       <c r="G5" s="16">
-        <v>44116</v>
+        <v>44104</v>
       </c>
       <c r="H5" s="6" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="I5" s="6" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="J5" s="6" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="K5" s="6" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="L5" s="6" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="M5" s="6" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="N5" s="6" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>25</v>
+        <v>43</v>
       </c>
       <c r="D6" s="15">
-        <v>44129.916666666664</v>
+        <v>44116.958333333336</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="F6" s="16">
-        <v>44105</v>
+        <v>44116</v>
       </c>
       <c r="G6" s="16">
-        <v>44135</v>
+        <v>44165</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="I6" s="6" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="J6" s="6" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="K6" s="6" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="L6" s="6" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="M6" s="6" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="N6" s="6" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B7" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="D7" s="15">
+        <v>44116.958333333336</v>
+      </c>
+      <c r="E7" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="C7" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="D7" s="15">
-        <v>43922.916666666664</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>23</v>
-      </c>
       <c r="F7" s="16">
-        <v>44109</v>
+        <v>44116</v>
       </c>
       <c r="G7" s="16">
-        <v>44135</v>
+        <v>44165</v>
       </c>
       <c r="H7" s="6" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="I7" s="6" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="J7" s="6" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="K7" s="6" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="L7" s="6" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="M7" s="6" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="N7" s="6" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B8" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C8" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="C8" s="14" t="s">
-        <v>28</v>
-      </c>
       <c r="D8" s="15">
-        <v>44109.625</v>
+        <v>44116.958333333336</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>21</v>
+        <v>45</v>
       </c>
       <c r="F8" s="16">
-        <v>44136</v>
+        <v>44116</v>
       </c>
       <c r="G8" s="16">
-        <v>44135</v>
+        <v>44165</v>
       </c>
       <c r="H8" s="6" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="I8" s="6" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="J8" s="6" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="K8" s="6" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="L8" s="6" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="M8" s="6" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="N8" s="6" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="D9" s="15">
-        <v>44110.583333333336</v>
+        <v>44116.958333333336</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>22</v>
+        <v>45</v>
       </c>
       <c r="F9" s="16">
-        <v>44168</v>
+        <v>44116</v>
       </c>
       <c r="G9" s="16">
-        <v>44135</v>
+        <v>44165</v>
       </c>
       <c r="H9" s="6" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="I9" s="6" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="J9" s="6" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="K9" s="6" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="L9" s="6" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="M9" s="6" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="N9" s="6" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="D10" s="15">
-        <v>43922.916666666664</v>
+        <v>44105.625</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>23</v>
+        <v>49</v>
       </c>
       <c r="F10" s="16">
-        <v>44109</v>
+        <v>44105</v>
       </c>
       <c r="G10" s="16">
         <v>44135</v>
       </c>
       <c r="H10" s="6" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="I10" s="6" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="J10" s="6" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="K10" s="6" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="L10" s="6" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="M10" s="6" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="N10" s="6" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
@@ -1872,12 +1856,6 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>Validacion!$A$2:$A$14</xm:f>
-          </x14:formula1>
-          <xm:sqref>A2:A45</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
             <xm:f>Validacion!$B$2:$B$14</xm:f>
           </x14:formula1>
           <xm:sqref>C2:C46</xm:sqref>
@@ -1887,6 +1865,12 @@
             <xm:f>Validacion!$C$2:$C$3</xm:f>
           </x14:formula1>
           <xm:sqref>H2:N53</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Señal de la promo" prompt="Valores posibles: EGSUR / EGNOR / MCLATAM / MCUSA / EE / FALATAM / FABRASIL / AMCSUR / AMCNORCOL / AMCLATAM AMCBRASIL_x000a__AMCNETWORKS (para promos corporativas)_x000a_OFFAIR (para promos que no salen al aire)_x000a_">
+          <x14:formula1>
+            <xm:f>Validacion!$A$2:$A$14</xm:f>
+          </x14:formula1>
+          <xm:sqref>A2:A50</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1898,8 +1882,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1916,18 +1900,18 @@
         <v>2</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="B2" s="19" t="s">
-        <v>36</v>
+        <v>41</v>
+      </c>
+      <c r="B2" s="18" t="s">
+        <v>32</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
@@ -1940,11 +1924,11 @@
       <c r="A3" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="19" t="s">
-        <v>35</v>
+      <c r="B3" s="18" t="s">
+        <v>31</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
@@ -1958,7 +1942,7 @@
         <v>17</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C4" s="6"/>
     </row>
@@ -1966,8 +1950,8 @@
       <c r="A5" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="8" t="s">
-        <v>24</v>
+      <c r="B5" s="17" t="s">
+        <v>36</v>
       </c>
       <c r="C5" s="6"/>
     </row>
@@ -1976,7 +1960,7 @@
         <v>15</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C6" s="6"/>
     </row>
@@ -1984,20 +1968,17 @@
       <c r="A7" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="17" t="s">
-        <v>31</v>
+      <c r="B7" s="8" t="s">
+        <v>22</v>
       </c>
       <c r="C7" s="6"/>
-      <c r="D7" t="s">
-        <v>48</v>
-      </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="8" t="s">
-        <v>26</v>
+      <c r="B8" s="18" t="s">
+        <v>43</v>
       </c>
       <c r="C8" s="6"/>
     </row>
@@ -2005,8 +1986,8 @@
       <c r="A9" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="8" t="s">
-        <v>28</v>
+      <c r="B9" s="18" t="s">
+        <v>23</v>
       </c>
       <c r="C9" s="6"/>
     </row>
@@ -2014,8 +1995,8 @@
       <c r="A10" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="8" t="s">
-        <v>27</v>
+      <c r="B10" s="18" t="s">
+        <v>25</v>
       </c>
       <c r="C10" s="6"/>
     </row>
@@ -2023,8 +2004,8 @@
       <c r="A11" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="17" t="s">
-        <v>30</v>
+      <c r="B11" s="18" t="s">
+        <v>24</v>
       </c>
       <c r="C11" s="6"/>
     </row>
@@ -2033,7 +2014,7 @@
         <v>12</v>
       </c>
       <c r="B12" s="18" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="C12" s="6"/>
     </row>
@@ -2041,9 +2022,7 @@
       <c r="A13" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="18" t="s">
-        <v>47</v>
-      </c>
+      <c r="B13" s="17"/>
       <c r="C13" s="6"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
@@ -2052,6 +2031,21 @@
       </c>
       <c r="B14" s="9"/>
       <c r="C14" s="6"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B15" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B16" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B17" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="3"/>
@@ -2067,8 +2061,8 @@
       <c r="C22" s="3"/>
     </row>
   </sheetData>
-  <sortState ref="A2:A14">
-    <sortCondition ref="A2"/>
+  <sortState ref="B2:B13">
+    <sortCondition ref="B13"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Alertas y unidecode agregadas. terminado AMC
</commit_message>
<xml_diff>
--- a/input.xlsx
+++ b/input.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="80" yWindow="460" windowWidth="23860" windowHeight="10140" tabRatio="500"/>
+    <workbookView xWindow="5440" yWindow="460" windowWidth="23860" windowHeight="10140" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="52">
   <si>
     <t>showFeed</t>
   </si>
@@ -192,9 +192,6 @@
     <t>NO</t>
   </si>
   <si>
-    <t>EPISODICAS</t>
-  </si>
-  <si>
     <t>Promo Mediodia se vende como GEN</t>
   </si>
   <si>
@@ -248,16 +245,25 @@
     <t>lunes</t>
   </si>
   <si>
-    <t>BOTTOMLESS BRUNCH AT COLEMAN TEMP 2</t>
-  </si>
-  <si>
-    <t>FEAR THE WALKING DEAD S6A</t>
-  </si>
-  <si>
     <t>GUARDIANES DE TRADICION</t>
   </si>
   <si>
     <t>MARTES</t>
+  </si>
+  <si>
+    <t>128705-NOS4A2 ON THE NEXT 205 A 206</t>
+  </si>
+  <si>
+    <t>EPISODICA</t>
+  </si>
+  <si>
+    <t>LA VIDA OLALÁ</t>
+  </si>
+  <si>
+    <t>GAHWOSKA</t>
+  </si>
+  <si>
+    <t>MIÉRCOLES</t>
   </si>
 </sst>
 </file>
@@ -696,10 +702,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N53"/>
+  <dimension ref="A1:N49"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -743,10 +749,10 @@
         <v>29</v>
       </c>
       <c r="H1" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="I1" s="19" t="s">
         <v>39</v>
-      </c>
-      <c r="I1" s="19" t="s">
-        <v>40</v>
       </c>
       <c r="J1" s="11" t="s">
         <v>3</v>
@@ -766,31 +772,31 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>46</v>
+        <v>14</v>
+      </c>
+      <c r="B2" t="s">
+        <v>49</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="D2" s="15">
-        <v>44109.916666666664</v>
+        <v>44116.958333333336</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F2" s="16">
-        <v>44080</v>
+        <v>44116</v>
       </c>
       <c r="G2" s="16">
-        <v>44104</v>
+        <v>44165</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J2" s="6" t="s">
         <v>35</v>
@@ -810,31 +816,31 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>46</v>
+        <v>12</v>
+      </c>
+      <c r="B3" t="s">
+        <v>47</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="D3" s="15">
-        <v>44109.916666666664</v>
+        <v>44116.958333333336</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F3" s="16">
-        <v>44080</v>
+        <v>44116</v>
       </c>
       <c r="G3" s="16">
-        <v>44104</v>
+        <v>44165</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I3" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J3" s="6" t="s">
         <v>35</v>
@@ -854,31 +860,31 @@
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>46</v>
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
+        <v>50</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="D4" s="15">
-        <v>44109.916666666664</v>
+        <v>44116.958333333336</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="F4" s="16">
-        <v>44080</v>
+        <v>44116</v>
       </c>
       <c r="G4" s="16">
-        <v>44104</v>
+        <v>44165</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I4" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J4" s="6" t="s">
         <v>35</v>
@@ -898,31 +904,31 @@
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>46</v>
+        <v>9</v>
+      </c>
+      <c r="B5" t="s">
+        <v>47</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>22</v>
+        <v>48</v>
       </c>
       <c r="D5" s="15">
-        <v>44109.916666666664</v>
+        <v>44116.958333333336</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F5" s="16">
-        <v>44080</v>
+        <v>44116</v>
       </c>
       <c r="G5" s="16">
-        <v>44104</v>
+        <v>44165</v>
       </c>
       <c r="H5" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I5" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J5" s="6" t="s">
         <v>35</v>
@@ -942,31 +948,31 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="D6" s="15">
-        <v>44116.958333333336</v>
+        <v>44105.625</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="F6" s="16">
-        <v>44116</v>
+        <v>44105</v>
       </c>
       <c r="G6" s="16">
-        <v>44165</v>
+        <v>44135</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I6" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J6" s="6" t="s">
         <v>35</v>
@@ -985,180 +991,68 @@
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A7" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="C7" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="D7" s="15">
-        <v>44116.958333333336</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="F7" s="16">
-        <v>44116</v>
-      </c>
-      <c r="G7" s="16">
-        <v>44165</v>
-      </c>
-      <c r="H7" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="I7" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="J7" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="K7" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="L7" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="M7" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="N7" s="6" t="s">
-        <v>35</v>
-      </c>
+      <c r="A7" s="6"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="6"/>
+      <c r="J7" s="6"/>
+      <c r="K7" s="6"/>
+      <c r="L7" s="6"/>
+      <c r="M7" s="6"/>
+      <c r="N7" s="6"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A8" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="C8" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="D8" s="15">
-        <v>44116.958333333336</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="F8" s="16">
-        <v>44116</v>
-      </c>
-      <c r="G8" s="16">
-        <v>44165</v>
-      </c>
-      <c r="H8" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="I8" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="J8" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="K8" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="L8" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="M8" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="N8" s="6" t="s">
-        <v>35</v>
-      </c>
+      <c r="A8" s="6"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="6"/>
+      <c r="K8" s="6"/>
+      <c r="L8" s="6"/>
+      <c r="M8" s="6"/>
+      <c r="N8" s="6"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A9" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="C9" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="D9" s="15">
-        <v>44116.958333333336</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="F9" s="16">
-        <v>44116</v>
-      </c>
-      <c r="G9" s="16">
-        <v>44165</v>
-      </c>
-      <c r="H9" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="I9" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="J9" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="K9" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="L9" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="M9" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="N9" s="6" t="s">
-        <v>35</v>
-      </c>
+      <c r="A9" s="6"/>
+      <c r="B9" s="6"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="6"/>
+      <c r="K9" s="6"/>
+      <c r="L9" s="6"/>
+      <c r="M9" s="6"/>
+      <c r="N9" s="6"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A10" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="C10" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="D10" s="15">
-        <v>44105.625</v>
-      </c>
-      <c r="E10" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="F10" s="16">
-        <v>44105</v>
-      </c>
-      <c r="G10" s="16">
-        <v>44135</v>
-      </c>
-      <c r="H10" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="I10" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="J10" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="K10" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="L10" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="M10" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="N10" s="6" t="s">
-        <v>35</v>
-      </c>
+      <c r="A10" s="6"/>
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="6"/>
+      <c r="K10" s="6"/>
+      <c r="L10" s="6"/>
+      <c r="M10" s="6"/>
+      <c r="N10" s="6"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" s="6"/>
@@ -1784,70 +1678,6 @@
       <c r="M49" s="6"/>
       <c r="N49" s="6"/>
     </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A50" s="6"/>
-      <c r="B50" s="6"/>
-      <c r="C50" s="6"/>
-      <c r="D50" s="6"/>
-      <c r="E50" s="6"/>
-      <c r="F50" s="6"/>
-      <c r="G50" s="6"/>
-      <c r="H50" s="6"/>
-      <c r="I50" s="6"/>
-      <c r="J50" s="6"/>
-      <c r="K50" s="6"/>
-      <c r="L50" s="6"/>
-      <c r="M50" s="6"/>
-      <c r="N50" s="6"/>
-    </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A51" s="6"/>
-      <c r="B51" s="6"/>
-      <c r="C51" s="6"/>
-      <c r="D51" s="6"/>
-      <c r="E51" s="6"/>
-      <c r="F51" s="6"/>
-      <c r="G51" s="6"/>
-      <c r="H51" s="6"/>
-      <c r="I51" s="6"/>
-      <c r="J51" s="6"/>
-      <c r="K51" s="6"/>
-      <c r="L51" s="6"/>
-      <c r="M51" s="6"/>
-      <c r="N51" s="6"/>
-    </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A52" s="6"/>
-      <c r="B52" s="6"/>
-      <c r="C52" s="6"/>
-      <c r="D52" s="6"/>
-      <c r="E52" s="6"/>
-      <c r="F52" s="6"/>
-      <c r="G52" s="6"/>
-      <c r="H52" s="6"/>
-      <c r="I52" s="6"/>
-      <c r="J52" s="6"/>
-      <c r="K52" s="6"/>
-      <c r="L52" s="6"/>
-      <c r="M52" s="6"/>
-      <c r="N52" s="6"/>
-    </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A53" s="6"/>
-      <c r="B53" s="6"/>
-      <c r="C53" s="6"/>
-      <c r="D53" s="6"/>
-      <c r="E53" s="6"/>
-      <c r="F53" s="6"/>
-      <c r="G53" s="6"/>
-      <c r="H53" s="6"/>
-      <c r="I53" s="6"/>
-      <c r="J53" s="6"/>
-      <c r="K53" s="6"/>
-      <c r="L53" s="6"/>
-      <c r="M53" s="6"/>
-      <c r="N53" s="6"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1858,19 +1688,19 @@
           <x14:formula1>
             <xm:f>Validacion!$B$2:$B$14</xm:f>
           </x14:formula1>
-          <xm:sqref>C2:C46</xm:sqref>
+          <xm:sqref>C2:C42</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Validacion!$C$2:$C$3</xm:f>
           </x14:formula1>
-          <xm:sqref>H2:N53</xm:sqref>
+          <xm:sqref>H2:N49</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Señal de la promo" prompt="Valores posibles: EGSUR / EGNOR / MCLATAM / MCUSA / EE / FALATAM / FABRASIL / AMCSUR / AMCNORCOL / AMCLATAM AMCBRASIL_x000a__AMCNETWORKS (para promos corporativas)_x000a_OFFAIR (para promos que no salen al aire)_x000a_">
           <x14:formula1>
             <xm:f>Validacion!$A$2:$A$14</xm:f>
           </x14:formula1>
-          <xm:sqref>A2:A50</xm:sqref>
+          <xm:sqref>A2:A46</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1883,7 +1713,7 @@
   <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1905,7 +1735,7 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B2" s="18" t="s">
         <v>32</v>
@@ -1928,7 +1758,7 @@
         <v>31</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
@@ -1951,7 +1781,7 @@
         <v>16</v>
       </c>
       <c r="B5" s="17" t="s">
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="C5" s="6"/>
     </row>
@@ -1978,7 +1808,7 @@
         <v>11</v>
       </c>
       <c r="B8" s="18" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C8" s="6"/>
     </row>
@@ -2034,17 +1864,17 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
AMC*Feeds__Timestamp en name file__nuevo input
</commit_message>
<xml_diff>
--- a/input.xlsx
+++ b/input.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="5440" yWindow="460" windowWidth="23860" windowHeight="10140" tabRatio="500"/>
+    <workbookView xWindow="7360" yWindow="460" windowWidth="23860" windowHeight="10140" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="53">
   <si>
     <t>showFeed</t>
   </si>
@@ -198,6 +198,59 @@
     <t>SI</t>
   </si>
   <si>
+    <t>Promo Maraton se vende como Puntual</t>
+  </si>
+  <si>
+    <t>GEN_SERIES</t>
+  </si>
+  <si>
+    <t>GEN_SERIES es para las promos genéricas de series de AMC</t>
+  </si>
+  <si>
+    <t>lunes</t>
+  </si>
+  <si>
+    <t>GUARDIANES DE TRADICION</t>
+  </si>
+  <si>
+    <t>MARTES</t>
+  </si>
+  <si>
+    <t>128705-NOS4A2 ON THE NEXT 205 A 206</t>
+  </si>
+  <si>
+    <t>EPISODICA</t>
+  </si>
+  <si>
+    <t>LA VIDA OLALÁ</t>
+  </si>
+  <si>
+    <t>MIÉRCOLES</t>
+  </si>
+  <si>
+    <t>AMC*4FEEDS</t>
+  </si>
+  <si>
+    <t>OTRAS</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">dstChi
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Chile adelanta la hora? 
+(Abril a Septiembre)</t>
+    </r>
+  </si>
+  <si>
     <r>
       <t xml:space="preserve">dstMex
 </t>
@@ -210,60 +263,12 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>MEX adelanta la hora?</t>
+      <t>MEX adelanta la hora? 
+(Abril a Octubre)</t>
     </r>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">dstChi
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Chile adelanta la hora?</t>
-    </r>
-  </si>
-  <si>
-    <t>_AMCNETWORKS</t>
-  </si>
-  <si>
-    <t>Promo Maraton se vende como Puntual</t>
-  </si>
-  <si>
-    <t>GEN_SERIES</t>
-  </si>
-  <si>
-    <t>GEN_SERIES es para las promos genéricas de series de AMC</t>
-  </si>
-  <si>
-    <t>lunes</t>
-  </si>
-  <si>
-    <t>GUARDIANES DE TRADICION</t>
-  </si>
-  <si>
-    <t>MARTES</t>
-  </si>
-  <si>
-    <t>128705-NOS4A2 ON THE NEXT 205 A 206</t>
-  </si>
-  <si>
-    <t>EPISODICA</t>
-  </si>
-  <si>
-    <t>LA VIDA OLALÁ</t>
-  </si>
-  <si>
-    <t>GAHWOSKA</t>
-  </si>
-  <si>
-    <t>MIÉRCOLES</t>
+    <t>walking dead again and again</t>
   </si>
 </sst>
 </file>
@@ -705,19 +710,19 @@
   <dimension ref="A1:N49"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.6640625" customWidth="1"/>
     <col min="2" max="2" width="41.6640625" customWidth="1"/>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="27.83203125" customWidth="1"/>
     <col min="5" max="5" width="24.6640625" customWidth="1"/>
     <col min="6" max="6" width="15.1640625" customWidth="1"/>
     <col min="7" max="7" width="15" customWidth="1"/>
-    <col min="8" max="8" width="12.33203125" customWidth="1"/>
+    <col min="8" max="8" width="14.6640625" customWidth="1"/>
     <col min="9" max="9" width="17.5" customWidth="1"/>
     <col min="10" max="10" width="15.5" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12" bestFit="1" customWidth="1"/>
@@ -749,10 +754,10 @@
         <v>29</v>
       </c>
       <c r="H1" s="12" t="s">
-        <v>38</v>
+        <v>51</v>
       </c>
       <c r="I1" s="19" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="J1" s="11" t="s">
         <v>3</v>
@@ -772,19 +777,19 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>14</v>
+        <v>48</v>
       </c>
       <c r="B2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="D2" s="15">
         <v>44116.958333333336</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="F2" s="16">
         <v>44116</v>
@@ -816,19 +821,19 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>12</v>
+        <v>48</v>
       </c>
       <c r="B3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="D3" s="15">
         <v>44116.958333333336</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="F3" s="16">
         <v>44116</v>
@@ -860,19 +865,19 @@
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
-        <v>13</v>
+        <v>48</v>
       </c>
       <c r="B4" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="D4" s="15">
         <v>44116.958333333336</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="F4" s="16">
         <v>44116</v>
@@ -907,16 +912,16 @@
         <v>9</v>
       </c>
       <c r="B5" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D5" s="15">
         <v>44116.958333333336</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="F5" s="16">
         <v>44116</v>
@@ -951,7 +956,7 @@
         <v>11</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C6" s="14" t="s">
         <v>31</v>
@@ -960,7 +965,7 @@
         <v>44105.625</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="F6" s="16">
         <v>44105</v>
@@ -1686,7 +1691,7 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>Validacion!$B$2:$B$14</xm:f>
+            <xm:f>Validacion!$B$2:$B$15</xm:f>
           </x14:formula1>
           <xm:sqref>C2:C42</xm:sqref>
         </x14:dataValidation>
@@ -1698,7 +1703,7 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Señal de la promo" prompt="Valores posibles: EGSUR / EGNOR / MCLATAM / MCUSA / EE / FALATAM / FABRASIL / AMCSUR / AMCNORCOL / AMCLATAM AMCBRASIL_x000a__AMCNETWORKS (para promos corporativas)_x000a_OFFAIR (para promos que no salen al aire)_x000a_">
           <x14:formula1>
-            <xm:f>Validacion!$A$2:$A$14</xm:f>
+            <xm:f>Validacion!$A$2:$A$15</xm:f>
           </x14:formula1>
           <xm:sqref>A2:A46</xm:sqref>
         </x14:dataValidation>
@@ -1710,10 +1715,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I22"/>
+  <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1735,7 +1740,7 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="B2" s="18" t="s">
         <v>32</v>
@@ -1781,7 +1786,7 @@
         <v>16</v>
       </c>
       <c r="B5" s="17" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C5" s="6"/>
     </row>
@@ -1808,7 +1813,7 @@
         <v>11</v>
       </c>
       <c r="B8" s="18" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C8" s="6"/>
     </row>
@@ -1859,40 +1864,47 @@
       <c r="A14" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="B14" s="9"/>
+      <c r="B14" s="17"/>
       <c r="C14" s="6"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B15" t="s">
-        <v>43</v>
-      </c>
+      <c r="A15" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="B15" s="9"/>
+      <c r="C15" s="6"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A21" s="3"/>
-      <c r="B21" s="3"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="3"/>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B18" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A23" s="3"/>
+      <c r="B23" s="3"/>
+      <c r="C23" s="3"/>
     </row>
   </sheetData>
-  <sortState ref="B2:B13">
-    <sortCondition ref="B13"/>
+  <sortState ref="A2:A15">
+    <sortCondition ref="A15"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
agregada duracion, conversor a TC
</commit_message>
<xml_diff>
--- a/input.xlsx
+++ b/input.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="7360" yWindow="460" windowWidth="23860" windowHeight="10140" tabRatio="500"/>
+    <workbookView xWindow="2860" yWindow="460" windowWidth="29680" windowHeight="12000" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -28,14 +28,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="55">
   <si>
     <t>showFeed</t>
   </si>
   <si>
-    <t>genDateStr</t>
-  </si>
-  <si>
     <t>promoPckg</t>
   </si>
   <si>
@@ -115,38 +112,6 @@
   </si>
   <si>
     <t>Booleans</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">endDate
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Fecha en cuando deja de rotar la promo</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">genStartDate
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Fecha en cuando empieza a rotar la promo generica</t>
-    </r>
   </si>
   <si>
     <t>CAPS ESTRENO</t>
@@ -219,9 +184,6 @@
     <t>128705-NOS4A2 ON THE NEXT 205 A 206</t>
   </si>
   <si>
-    <t>EPISODICA</t>
-  </si>
-  <si>
     <t>LA VIDA OLALÁ</t>
   </si>
   <si>
@@ -270,12 +232,120 @@
   <si>
     <t>walking dead again and again</t>
   </si>
+  <si>
+    <r>
+      <t xml:space="preserve">genDateStr
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>fecha de venta para la promo GENÉRICA</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">endDate
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Fecha en cuando </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>deja de rotar</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> la promo</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">genStartDate
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Fecha en cuando </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>empieza a rotar</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> la promo generica</t>
+    </r>
+  </si>
+  <si>
+    <t>PELI DEL MES</t>
+  </si>
+  <si>
+    <t>Para las EPISODICAS, usamos genericas de AMC (dia / mañana / esta noche)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">duration
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Si es 30 seg o no sabes, dejar en blanco</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -320,13 +390,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="12"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <i/>
       <sz val="10"/>
       <name val="Calibri"/>
@@ -351,6 +414,19 @@
       <sz val="12"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri (Cuerpo)"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -400,7 +476,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -416,14 +492,11 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -707,10 +780,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N49"/>
+  <dimension ref="A1:O49"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -718,284 +791,245 @@
     <col min="1" max="1" width="13.6640625" customWidth="1"/>
     <col min="2" max="2" width="41.6640625" customWidth="1"/>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.83203125" customWidth="1"/>
-    <col min="5" max="5" width="24.6640625" customWidth="1"/>
-    <col min="6" max="6" width="15.1640625" customWidth="1"/>
-    <col min="7" max="7" width="15" customWidth="1"/>
-    <col min="8" max="8" width="14.6640625" customWidth="1"/>
-    <col min="9" max="9" width="17.5" customWidth="1"/>
-    <col min="10" max="10" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="5.33203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="7.1640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.83203125" customWidth="1"/>
+    <col min="5" max="5" width="27.83203125" customWidth="1"/>
+    <col min="6" max="6" width="24.6640625" customWidth="1"/>
+    <col min="7" max="7" width="15.1640625" customWidth="1"/>
+    <col min="8" max="8" width="15" customWidth="1"/>
+    <col min="9" max="9" width="14.6640625" customWidth="1"/>
+    <col min="10" max="10" width="17.5" customWidth="1"/>
+    <col min="11" max="11" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="1" customFormat="1" ht="99" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" s="1" customFormat="1" ht="99" x14ac:dyDescent="0.2">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="F1" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="G1" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="H1" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="I1" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="J1" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="K1" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="L1" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="M1" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="N1" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="O1" s="11" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A2" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="13"/>
+      <c r="E2" s="14">
+        <v>44116.958333333336</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="G2" s="15">
+        <v>44116</v>
+      </c>
+      <c r="H2" s="15">
+        <v>44165</v>
+      </c>
+      <c r="I2" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="C1" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="E1" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="G1" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="H1" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="I1" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="J1" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="K1" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="L1" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="M1" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="N1" s="11" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A2" s="6" t="s">
+      <c r="J2" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="K2" s="6"/>
+      <c r="L2" s="6"/>
+      <c r="M2" s="6"/>
+      <c r="N2" s="6"/>
+      <c r="O2" s="6"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A3" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="B3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" s="13"/>
+      <c r="E3" s="14">
+        <v>44116.958333333336</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="G3" s="15">
+        <v>44116</v>
+      </c>
+      <c r="H3" s="15">
+        <v>44165</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="J3" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="K3" s="6"/>
+      <c r="L3" s="6"/>
+      <c r="M3" s="6"/>
+      <c r="N3" s="6"/>
+      <c r="O3" s="6"/>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A4" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="B4" t="s">
         <v>48</v>
       </c>
-      <c r="B2" t="s">
-        <v>46</v>
-      </c>
-      <c r="C2" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="D2" s="15">
+      <c r="C4" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="D4" s="13">
+        <v>60</v>
+      </c>
+      <c r="E4" s="14">
         <v>44116.958333333336</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="F4" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="G4" s="15">
+        <v>44116</v>
+      </c>
+      <c r="H4" s="15">
+        <v>44165</v>
+      </c>
+      <c r="I4" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="J4" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="K4" s="6"/>
+      <c r="L4" s="6"/>
+      <c r="M4" s="6"/>
+      <c r="N4" s="6"/>
+      <c r="O4" s="6"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A5" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
         <v>41</v>
       </c>
-      <c r="F2" s="16">
+      <c r="C5" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" s="13"/>
+      <c r="E5" s="14">
+        <v>44116.958333333336</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="G5" s="15">
         <v>44116</v>
       </c>
-      <c r="G2" s="16">
+      <c r="H5" s="15">
         <v>44165</v>
       </c>
-      <c r="H2" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="I2" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="J2" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="K2" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="L2" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="M2" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="N2" s="6" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A3" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="B3" t="s">
-        <v>44</v>
-      </c>
-      <c r="C3" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="D3" s="15">
-        <v>44116.958333333336</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="F3" s="16">
-        <v>44116</v>
-      </c>
-      <c r="G3" s="16">
-        <v>44165</v>
-      </c>
-      <c r="H3" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="I3" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="J3" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="K3" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="L3" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="M3" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="N3" s="6" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A4" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="B4" t="s">
-        <v>52</v>
-      </c>
-      <c r="C4" s="14" t="s">
+      <c r="I5" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="J5" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="K5" s="6"/>
+      <c r="L5" s="6"/>
+      <c r="M5" s="6"/>
+      <c r="N5" s="6"/>
+      <c r="O5" s="6"/>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A6" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="D4" s="15">
-        <v>44116.958333333336</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="F4" s="16">
-        <v>44116</v>
-      </c>
-      <c r="G4" s="16">
-        <v>44165</v>
-      </c>
-      <c r="H4" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="I4" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="J4" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="K4" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="L4" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="M4" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="N4" s="6" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A5" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" t="s">
-        <v>44</v>
-      </c>
-      <c r="C5" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="D5" s="15">
-        <v>44116.958333333336</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="F5" s="16">
-        <v>44116</v>
-      </c>
-      <c r="G5" s="16">
-        <v>44165</v>
-      </c>
-      <c r="H5" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="I5" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="J5" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="K5" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="L5" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="M5" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="N5" s="6" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A6" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="C6" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="D6" s="15">
+      <c r="C6" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" s="13"/>
+      <c r="E6" s="14">
         <v>44105.625</v>
       </c>
-      <c r="E6" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="F6" s="16">
+      <c r="F6" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="G6" s="15">
         <v>44105</v>
       </c>
-      <c r="G6" s="16">
-        <v>44135</v>
-      </c>
-      <c r="H6" s="6" t="s">
-        <v>37</v>
+      <c r="H6" s="15">
+        <v>44105</v>
       </c>
       <c r="I6" s="6" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="J6" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="K6" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="L6" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="M6" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="N6" s="6" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+        <v>34</v>
+      </c>
+      <c r="K6" s="6"/>
+      <c r="L6" s="6"/>
+      <c r="M6" s="6"/>
+      <c r="N6" s="6"/>
+      <c r="O6" s="6"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" s="6"/>
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
@@ -1010,8 +1044,9 @@
       <c r="L7" s="6"/>
       <c r="M7" s="6"/>
       <c r="N7" s="6"/>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O7" s="6"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" s="6"/>
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
@@ -1026,8 +1061,9 @@
       <c r="L8" s="6"/>
       <c r="M8" s="6"/>
       <c r="N8" s="6"/>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O8" s="6"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" s="6"/>
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
@@ -1042,8 +1078,9 @@
       <c r="L9" s="6"/>
       <c r="M9" s="6"/>
       <c r="N9" s="6"/>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O9" s="6"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" s="6"/>
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
@@ -1058,8 +1095,9 @@
       <c r="L10" s="6"/>
       <c r="M10" s="6"/>
       <c r="N10" s="6"/>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O10" s="6"/>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" s="6"/>
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
@@ -1074,8 +1112,9 @@
       <c r="L11" s="6"/>
       <c r="M11" s="6"/>
       <c r="N11" s="6"/>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O11" s="6"/>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
@@ -1090,8 +1129,9 @@
       <c r="L12" s="6"/>
       <c r="M12" s="6"/>
       <c r="N12" s="6"/>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O12" s="6"/>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" s="6"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -1106,8 +1146,9 @@
       <c r="L13" s="6"/>
       <c r="M13" s="6"/>
       <c r="N13" s="6"/>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O13" s="6"/>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14" s="6"/>
       <c r="B14" s="6"/>
       <c r="C14" s="6"/>
@@ -1122,8 +1163,9 @@
       <c r="L14" s="6"/>
       <c r="M14" s="6"/>
       <c r="N14" s="6"/>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O14" s="6"/>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15" s="6"/>
       <c r="B15" s="6"/>
       <c r="C15" s="6"/>
@@ -1138,8 +1180,9 @@
       <c r="L15" s="6"/>
       <c r="M15" s="6"/>
       <c r="N15" s="6"/>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O15" s="6"/>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16" s="6"/>
       <c r="B16" s="6"/>
       <c r="C16" s="6"/>
@@ -1154,8 +1197,9 @@
       <c r="L16" s="6"/>
       <c r="M16" s="6"/>
       <c r="N16" s="6"/>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O16" s="6"/>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A17" s="6"/>
       <c r="B17" s="6"/>
       <c r="C17" s="6"/>
@@ -1170,8 +1214,9 @@
       <c r="L17" s="6"/>
       <c r="M17" s="6"/>
       <c r="N17" s="6"/>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O17" s="6"/>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A18" s="6"/>
       <c r="B18" s="6"/>
       <c r="C18" s="6"/>
@@ -1186,8 +1231,9 @@
       <c r="L18" s="6"/>
       <c r="M18" s="6"/>
       <c r="N18" s="6"/>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O18" s="6"/>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A19" s="6"/>
       <c r="B19" s="6"/>
       <c r="C19" s="6"/>
@@ -1202,8 +1248,9 @@
       <c r="L19" s="6"/>
       <c r="M19" s="6"/>
       <c r="N19" s="6"/>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O19" s="6"/>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A20" s="6"/>
       <c r="B20" s="6"/>
       <c r="C20" s="6"/>
@@ -1218,8 +1265,9 @@
       <c r="L20" s="6"/>
       <c r="M20" s="6"/>
       <c r="N20" s="6"/>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O20" s="6"/>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A21" s="6"/>
       <c r="B21" s="6"/>
       <c r="C21" s="6"/>
@@ -1234,8 +1282,9 @@
       <c r="L21" s="6"/>
       <c r="M21" s="6"/>
       <c r="N21" s="6"/>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O21" s="6"/>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A22" s="6"/>
       <c r="B22" s="6"/>
       <c r="C22" s="6"/>
@@ -1250,8 +1299,9 @@
       <c r="L22" s="6"/>
       <c r="M22" s="6"/>
       <c r="N22" s="6"/>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O22" s="6"/>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A23" s="6"/>
       <c r="B23" s="6"/>
       <c r="C23" s="6"/>
@@ -1266,8 +1316,9 @@
       <c r="L23" s="6"/>
       <c r="M23" s="6"/>
       <c r="N23" s="6"/>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O23" s="6"/>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A24" s="6"/>
       <c r="B24" s="6"/>
       <c r="C24" s="6"/>
@@ -1282,8 +1333,9 @@
       <c r="L24" s="6"/>
       <c r="M24" s="6"/>
       <c r="N24" s="6"/>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O24" s="6"/>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A25" s="6"/>
       <c r="B25" s="6"/>
       <c r="C25" s="6"/>
@@ -1298,8 +1350,9 @@
       <c r="L25" s="6"/>
       <c r="M25" s="6"/>
       <c r="N25" s="6"/>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O25" s="6"/>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A26" s="6"/>
       <c r="B26" s="6"/>
       <c r="C26" s="6"/>
@@ -1314,8 +1367,9 @@
       <c r="L26" s="6"/>
       <c r="M26" s="6"/>
       <c r="N26" s="6"/>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O26" s="6"/>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A27" s="6"/>
       <c r="B27" s="6"/>
       <c r="C27" s="6"/>
@@ -1330,8 +1384,9 @@
       <c r="L27" s="6"/>
       <c r="M27" s="6"/>
       <c r="N27" s="6"/>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O27" s="6"/>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A28" s="6"/>
       <c r="B28" s="6"/>
       <c r="C28" s="6"/>
@@ -1346,8 +1401,9 @@
       <c r="L28" s="6"/>
       <c r="M28" s="6"/>
       <c r="N28" s="6"/>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O28" s="6"/>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A29" s="6"/>
       <c r="B29" s="6"/>
       <c r="C29" s="6"/>
@@ -1362,8 +1418,9 @@
       <c r="L29" s="6"/>
       <c r="M29" s="6"/>
       <c r="N29" s="6"/>
-    </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O29" s="6"/>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A30" s="6"/>
       <c r="B30" s="6"/>
       <c r="C30" s="6"/>
@@ -1378,8 +1435,9 @@
       <c r="L30" s="6"/>
       <c r="M30" s="6"/>
       <c r="N30" s="6"/>
-    </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O30" s="6"/>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A31" s="6"/>
       <c r="B31" s="6"/>
       <c r="C31" s="6"/>
@@ -1394,8 +1452,9 @@
       <c r="L31" s="6"/>
       <c r="M31" s="6"/>
       <c r="N31" s="6"/>
-    </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O31" s="6"/>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A32" s="6"/>
       <c r="B32" s="6"/>
       <c r="C32" s="6"/>
@@ -1410,8 +1469,9 @@
       <c r="L32" s="6"/>
       <c r="M32" s="6"/>
       <c r="N32" s="6"/>
-    </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O32" s="6"/>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A33" s="6"/>
       <c r="B33" s="6"/>
       <c r="C33" s="6"/>
@@ -1426,8 +1486,9 @@
       <c r="L33" s="6"/>
       <c r="M33" s="6"/>
       <c r="N33" s="6"/>
-    </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O33" s="6"/>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A34" s="6"/>
       <c r="B34" s="6"/>
       <c r="C34" s="6"/>
@@ -1442,8 +1503,9 @@
       <c r="L34" s="6"/>
       <c r="M34" s="6"/>
       <c r="N34" s="6"/>
-    </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O34" s="6"/>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A35" s="6"/>
       <c r="B35" s="6"/>
       <c r="C35" s="6"/>
@@ -1458,8 +1520,9 @@
       <c r="L35" s="6"/>
       <c r="M35" s="6"/>
       <c r="N35" s="6"/>
-    </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O35" s="6"/>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A36" s="6"/>
       <c r="B36" s="6"/>
       <c r="C36" s="6"/>
@@ -1474,8 +1537,9 @@
       <c r="L36" s="6"/>
       <c r="M36" s="6"/>
       <c r="N36" s="6"/>
-    </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O36" s="6"/>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A37" s="6"/>
       <c r="B37" s="6"/>
       <c r="C37" s="6"/>
@@ -1490,8 +1554,9 @@
       <c r="L37" s="6"/>
       <c r="M37" s="6"/>
       <c r="N37" s="6"/>
-    </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O37" s="6"/>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
@@ -1506,8 +1571,9 @@
       <c r="L38" s="6"/>
       <c r="M38" s="6"/>
       <c r="N38" s="6"/>
-    </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O38" s="6"/>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A39" s="6"/>
       <c r="B39" s="6"/>
       <c r="C39" s="6"/>
@@ -1522,8 +1588,9 @@
       <c r="L39" s="6"/>
       <c r="M39" s="6"/>
       <c r="N39" s="6"/>
-    </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O39" s="6"/>
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A40" s="6"/>
       <c r="B40" s="6"/>
       <c r="C40" s="6"/>
@@ -1538,8 +1605,9 @@
       <c r="L40" s="6"/>
       <c r="M40" s="6"/>
       <c r="N40" s="6"/>
-    </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O40" s="6"/>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A41" s="6"/>
       <c r="B41" s="6"/>
       <c r="C41" s="6"/>
@@ -1554,8 +1622,9 @@
       <c r="L41" s="6"/>
       <c r="M41" s="6"/>
       <c r="N41" s="6"/>
-    </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O41" s="6"/>
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A42" s="6"/>
       <c r="B42" s="6"/>
       <c r="C42" s="6"/>
@@ -1570,8 +1639,9 @@
       <c r="L42" s="6"/>
       <c r="M42" s="6"/>
       <c r="N42" s="6"/>
-    </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O42" s="6"/>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A43" s="6"/>
       <c r="B43" s="6"/>
       <c r="C43" s="6"/>
@@ -1586,8 +1656,9 @@
       <c r="L43" s="6"/>
       <c r="M43" s="6"/>
       <c r="N43" s="6"/>
-    </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O43" s="6"/>
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A44" s="6"/>
       <c r="B44" s="6"/>
       <c r="C44" s="6"/>
@@ -1602,8 +1673,9 @@
       <c r="L44" s="6"/>
       <c r="M44" s="6"/>
       <c r="N44" s="6"/>
-    </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O44" s="6"/>
+    </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A45" s="6"/>
       <c r="B45" s="6"/>
       <c r="C45" s="6"/>
@@ -1618,8 +1690,9 @@
       <c r="L45" s="6"/>
       <c r="M45" s="6"/>
       <c r="N45" s="6"/>
-    </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O45" s="6"/>
+    </row>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A46" s="6"/>
       <c r="B46" s="6"/>
       <c r="C46" s="6"/>
@@ -1634,8 +1707,9 @@
       <c r="L46" s="6"/>
       <c r="M46" s="6"/>
       <c r="N46" s="6"/>
-    </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O46" s="6"/>
+    </row>
+    <row r="47" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A47" s="6"/>
       <c r="B47" s="6"/>
       <c r="C47" s="6"/>
@@ -1650,8 +1724,9 @@
       <c r="L47" s="6"/>
       <c r="M47" s="6"/>
       <c r="N47" s="6"/>
-    </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O47" s="6"/>
+    </row>
+    <row r="48" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A48" s="6"/>
       <c r="B48" s="6"/>
       <c r="C48" s="6"/>
@@ -1666,8 +1741,9 @@
       <c r="L48" s="6"/>
       <c r="M48" s="6"/>
       <c r="N48" s="6"/>
-    </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O48" s="6"/>
+    </row>
+    <row r="49" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A49" s="6"/>
       <c r="B49" s="6"/>
       <c r="C49" s="6"/>
@@ -1682,8 +1758,17 @@
       <c r="L49" s="6"/>
       <c r="M49" s="6"/>
       <c r="N49" s="6"/>
+      <c r="O49" s="6"/>
     </row>
   </sheetData>
+  <dataValidations count="2">
+    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Error" error="La fecha de fin debe ser posterior a la fecha de inicio" sqref="H2:H49">
+      <formula1>G2</formula1>
+    </dataValidation>
+    <dataValidation type="whole" operator="greaterThanOrEqual" showInputMessage="1" showErrorMessage="1" sqref="D2:D49">
+      <formula1>1</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>
@@ -1697,9 +1782,9 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>Validacion!$C$2:$C$3</xm:f>
+            <xm:f>Validacion!$C$2:$C$4</xm:f>
           </x14:formula1>
-          <xm:sqref>H2:N49</xm:sqref>
+          <xm:sqref>I2:O49</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Señal de la promo" prompt="Valores posibles: EGSUR / EGNOR / MCLATAM / MCUSA / EE / FALATAM / FABRASIL / AMCSUR / AMCNORCOL / AMCLATAM AMCBRASIL_x000a__AMCNETWORKS (para promos corporativas)_x000a_OFFAIR (para promos que no salen al aire)_x000a_">
           <x14:formula1>
@@ -1718,7 +1803,7 @@
   <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1729,24 +1814,24 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="B2" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" s="7" t="s">
         <v>32</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>35</v>
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
@@ -1757,13 +1842,13 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="B3" s="18" t="s">
-        <v>31</v>
+        <v>17</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>28</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
@@ -1774,25 +1859,25 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C4" s="6"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" s="17" t="s">
-        <v>45</v>
+        <v>15</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>20</v>
       </c>
       <c r="C5" s="6"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B6" s="8" t="s">
         <v>21</v>
@@ -1801,92 +1886,97 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="B7" s="8" t="s">
-        <v>22</v>
+        <v>13</v>
+      </c>
+      <c r="B7" s="17" t="s">
+        <v>36</v>
       </c>
       <c r="C7" s="6"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" s="18" t="s">
-        <v>39</v>
+        <v>10</v>
+      </c>
+      <c r="B8" s="17" t="s">
+        <v>22</v>
       </c>
       <c r="C8" s="6"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" s="18" t="s">
-        <v>23</v>
+        <v>8</v>
+      </c>
+      <c r="B9" s="16" t="s">
+        <v>52</v>
       </c>
       <c r="C9" s="6"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="B10" s="18" t="s">
-        <v>25</v>
+        <v>18</v>
+      </c>
+      <c r="B10" s="17" t="s">
+        <v>24</v>
       </c>
       <c r="C10" s="6"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B11" s="18" t="s">
-        <v>24</v>
+        <v>9</v>
+      </c>
+      <c r="B11" s="17" t="s">
+        <v>23</v>
       </c>
       <c r="C11" s="6"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12" s="18" t="s">
-        <v>27</v>
+        <v>11</v>
+      </c>
+      <c r="B12" s="17" t="s">
+        <v>26</v>
       </c>
       <c r="C12" s="6"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B13" s="17"/>
+        <v>12</v>
+      </c>
+      <c r="B13" s="16"/>
       <c r="C13" s="6"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="B14" s="17"/>
+        <v>19</v>
+      </c>
+      <c r="B14" s="16"/>
       <c r="C14" s="6"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="7" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B15" s="9"/>
       <c r="C15" s="6"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
-        <v>38</v>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B19" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
@@ -1903,8 +1993,8 @@
       <c r="C23" s="3"/>
     </row>
   </sheetData>
-  <sortState ref="A2:A15">
-    <sortCondition ref="A15"/>
+  <sortState ref="B2:B15">
+    <sortCondition ref="B2"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
arreglado bug en listmaker
</commit_message>
<xml_diff>
--- a/input.xlsx
+++ b/input.xlsx
@@ -783,7 +783,7 @@
   <dimension ref="A1:O49"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -854,7 +854,7 @@
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>44</v>
+        <v>8</v>
       </c>
       <c r="B2" t="s">
         <v>42</v>
@@ -1803,7 +1803,7 @@
   <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
v2 de listmaker ya funcional
</commit_message>
<xml_diff>
--- a/input.xlsx
+++ b/input.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2860" yWindow="460" windowWidth="29680" windowHeight="12000" tabRatio="500"/>
+    <workbookView xWindow="2860" yWindow="460" windowWidth="16620" windowHeight="12000" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="58">
   <si>
     <t>showFeed</t>
   </si>
@@ -164,12 +164,6 @@
   </si>
   <si>
     <t>Promo Maraton se vende como Puntual</t>
-  </si>
-  <si>
-    <t>GEN_SERIES</t>
-  </si>
-  <si>
-    <t>GEN_SERIES es para las promos genéricas de series de AMC</t>
   </si>
   <si>
     <t>lunes</t>
@@ -323,9 +317,6 @@
     <t>PELI DEL MES</t>
   </si>
   <si>
-    <t>Para las EPISODICAS, usamos genericas de AMC (dia / mañana / esta noche)</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">duration
 </t>
@@ -339,6 +330,24 @@
       </rPr>
       <t>Si es 30 seg o no sabes, dejar en blanco</t>
     </r>
+  </si>
+  <si>
+    <t>GEN_AMC es para las promos genéricas de series de AMC, con Dia, mañana y hoy</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>GEN_AMC</t>
+  </si>
+  <si>
+    <t>Usa el genStartDate para poner la fecha y hora de la segunda pelicula</t>
+  </si>
+  <si>
+    <t>QUE PEDAZO DE PELI</t>
+  </si>
+  <si>
+    <t>nada</t>
   </si>
 </sst>
 </file>
@@ -783,7 +792,7 @@
   <dimension ref="A1:O49"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -816,25 +825,25 @@
         <v>1</v>
       </c>
       <c r="D1" s="18" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="E1" s="12" t="s">
         <v>30</v>
       </c>
       <c r="F1" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="G1" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="G1" s="18" t="s">
-        <v>51</v>
-      </c>
       <c r="H1" s="18" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="I1" s="12" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="J1" s="18" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="K1" s="11" t="s">
         <v>2</v>
@@ -857,7 +866,7 @@
         <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C2" s="13" t="s">
         <v>21</v>
@@ -867,7 +876,7 @@
         <v>44116.958333333336</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G2" s="15">
         <v>44116</v>
@@ -889,10 +898,10 @@
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C3" s="13" t="s">
         <v>25</v>
@@ -902,7 +911,7 @@
         <v>44116.958333333336</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G3" s="15">
         <v>44116</v>
@@ -924,13 +933,13 @@
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>36</v>
+        <v>54</v>
       </c>
       <c r="D4" s="13">
         <v>60</v>
@@ -939,7 +948,7 @@
         <v>44116.958333333336</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="G4" s="15">
         <v>44116</v>
@@ -964,7 +973,7 @@
         <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C5" s="13" t="s">
         <v>21</v>
@@ -974,7 +983,7 @@
         <v>44116.958333333336</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G5" s="15">
         <v>44116</v>
@@ -999,7 +1008,7 @@
         <v>10</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C6" s="13" t="s">
         <v>28</v>
@@ -1009,7 +1018,7 @@
         <v>44105.625</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G6" s="15">
         <v>44105</v>
@@ -1030,16 +1039,36 @@
       <c r="O6" s="6"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A7" s="6"/>
-      <c r="B7" s="6"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="6"/>
-      <c r="I7" s="6"/>
-      <c r="J7" s="6"/>
+      <c r="A7" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="D7" s="6">
+        <v>45</v>
+      </c>
+      <c r="E7" s="14">
+        <v>44125.916666666664</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="G7" s="14">
+        <v>44131.940972222219</v>
+      </c>
+      <c r="H7" s="15">
+        <v>44132</v>
+      </c>
+      <c r="I7" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="J7" s="6" t="s">
+        <v>34</v>
+      </c>
       <c r="K7" s="6"/>
       <c r="L7" s="6"/>
       <c r="M7" s="6"/>
@@ -1051,7 +1080,7 @@
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
       <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
+      <c r="E8" s="14"/>
       <c r="F8" s="6"/>
       <c r="G8" s="6"/>
       <c r="H8" s="6"/>
@@ -1068,7 +1097,7 @@
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
       <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
+      <c r="E9" s="14"/>
       <c r="F9" s="6"/>
       <c r="G9" s="6"/>
       <c r="H9" s="6"/>
@@ -1085,7 +1114,7 @@
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
       <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
+      <c r="E10" s="14"/>
       <c r="F10" s="6"/>
       <c r="G10" s="6"/>
       <c r="H10" s="6"/>
@@ -1102,7 +1131,7 @@
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
       <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
+      <c r="E11" s="14"/>
       <c r="F11" s="6"/>
       <c r="G11" s="6"/>
       <c r="H11" s="6"/>
@@ -1119,7 +1148,7 @@
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
       <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
+      <c r="E12" s="14"/>
       <c r="F12" s="6"/>
       <c r="G12" s="6"/>
       <c r="H12" s="6"/>
@@ -1136,7 +1165,7 @@
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
       <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
+      <c r="E13" s="14"/>
       <c r="F13" s="6"/>
       <c r="G13" s="6"/>
       <c r="H13" s="6"/>
@@ -1153,7 +1182,7 @@
       <c r="B14" s="6"/>
       <c r="C14" s="6"/>
       <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
+      <c r="E14" s="14"/>
       <c r="F14" s="6"/>
       <c r="G14" s="6"/>
       <c r="H14" s="6"/>
@@ -1170,7 +1199,7 @@
       <c r="B15" s="6"/>
       <c r="C15" s="6"/>
       <c r="D15" s="6"/>
-      <c r="E15" s="6"/>
+      <c r="E15" s="14"/>
       <c r="F15" s="6"/>
       <c r="G15" s="6"/>
       <c r="H15" s="6"/>
@@ -1187,7 +1216,7 @@
       <c r="B16" s="6"/>
       <c r="C16" s="6"/>
       <c r="D16" s="6"/>
-      <c r="E16" s="6"/>
+      <c r="E16" s="14"/>
       <c r="F16" s="6"/>
       <c r="G16" s="6"/>
       <c r="H16" s="6"/>
@@ -1204,7 +1233,7 @@
       <c r="B17" s="6"/>
       <c r="C17" s="6"/>
       <c r="D17" s="6"/>
-      <c r="E17" s="6"/>
+      <c r="E17" s="14"/>
       <c r="F17" s="6"/>
       <c r="G17" s="6"/>
       <c r="H17" s="6"/>
@@ -1221,7 +1250,7 @@
       <c r="B18" s="6"/>
       <c r="C18" s="6"/>
       <c r="D18" s="6"/>
-      <c r="E18" s="6"/>
+      <c r="E18" s="14"/>
       <c r="F18" s="6"/>
       <c r="G18" s="6"/>
       <c r="H18" s="6"/>
@@ -1238,7 +1267,7 @@
       <c r="B19" s="6"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
-      <c r="E19" s="6"/>
+      <c r="E19" s="14"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
       <c r="H19" s="6"/>
@@ -1255,7 +1284,7 @@
       <c r="B20" s="6"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
-      <c r="E20" s="6"/>
+      <c r="E20" s="14"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
       <c r="H20" s="6"/>
@@ -1803,7 +1832,7 @@
   <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1825,7 +1854,7 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B2" s="17" t="s">
         <v>29</v>
@@ -1889,7 +1918,7 @@
         <v>13</v>
       </c>
       <c r="B7" s="17" t="s">
-        <v>36</v>
+        <v>54</v>
       </c>
       <c r="C7" s="6"/>
     </row>
@@ -1906,8 +1935,8 @@
       <c r="A9" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="16" t="s">
-        <v>52</v>
+      <c r="B9" s="17" t="s">
+        <v>50</v>
       </c>
       <c r="C9" s="6"/>
     </row>
@@ -1954,14 +1983,14 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="7" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B15" s="9"/>
       <c r="C15" s="6"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
-        <v>37</v>
+        <v>52</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
@@ -1975,8 +2004,16 @@
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B19" t="s">
+      <c r="B19" s="3" t="s">
         <v>53</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B20" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="C20" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
List maker new (#1)
* funciona, entre alfileres.

* arreglado bug en listmaker

* v2 de listmaker ya funcional

* agregado suite de pruebas

Co-authored-by: Nac <cinelibr@gmail.com>
</commit_message>
<xml_diff>
--- a/input.xlsx
+++ b/input.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2860" yWindow="460" windowWidth="29680" windowHeight="12000" tabRatio="500"/>
+    <workbookView xWindow="2860" yWindow="460" windowWidth="16620" windowHeight="12000" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="58">
   <si>
     <t>showFeed</t>
   </si>
@@ -164,12 +164,6 @@
   </si>
   <si>
     <t>Promo Maraton se vende como Puntual</t>
-  </si>
-  <si>
-    <t>GEN_SERIES</t>
-  </si>
-  <si>
-    <t>GEN_SERIES es para las promos genéricas de series de AMC</t>
   </si>
   <si>
     <t>lunes</t>
@@ -323,9 +317,6 @@
     <t>PELI DEL MES</t>
   </si>
   <si>
-    <t>Para las EPISODICAS, usamos genericas de AMC (dia / mañana / esta noche)</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">duration
 </t>
@@ -339,6 +330,24 @@
       </rPr>
       <t>Si es 30 seg o no sabes, dejar en blanco</t>
     </r>
+  </si>
+  <si>
+    <t>GEN_AMC es para las promos genéricas de series de AMC, con Dia, mañana y hoy</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>GEN_AMC</t>
+  </si>
+  <si>
+    <t>Usa el genStartDate para poner la fecha y hora de la segunda pelicula</t>
+  </si>
+  <si>
+    <t>QUE PEDAZO DE PELI</t>
+  </si>
+  <si>
+    <t>nada</t>
   </si>
 </sst>
 </file>
@@ -783,7 +792,7 @@
   <dimension ref="A1:O49"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -816,25 +825,25 @@
         <v>1</v>
       </c>
       <c r="D1" s="18" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="E1" s="12" t="s">
         <v>30</v>
       </c>
       <c r="F1" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="G1" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="G1" s="18" t="s">
-        <v>51</v>
-      </c>
       <c r="H1" s="18" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="I1" s="12" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="J1" s="18" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="K1" s="11" t="s">
         <v>2</v>
@@ -854,10 +863,10 @@
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>44</v>
+        <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C2" s="13" t="s">
         <v>21</v>
@@ -867,7 +876,7 @@
         <v>44116.958333333336</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G2" s="15">
         <v>44116</v>
@@ -889,10 +898,10 @@
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C3" s="13" t="s">
         <v>25</v>
@@ -902,7 +911,7 @@
         <v>44116.958333333336</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G3" s="15">
         <v>44116</v>
@@ -924,13 +933,13 @@
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>36</v>
+        <v>54</v>
       </c>
       <c r="D4" s="13">
         <v>60</v>
@@ -939,7 +948,7 @@
         <v>44116.958333333336</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="G4" s="15">
         <v>44116</v>
@@ -964,7 +973,7 @@
         <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C5" s="13" t="s">
         <v>21</v>
@@ -974,7 +983,7 @@
         <v>44116.958333333336</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G5" s="15">
         <v>44116</v>
@@ -999,7 +1008,7 @@
         <v>10</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C6" s="13" t="s">
         <v>28</v>
@@ -1009,7 +1018,7 @@
         <v>44105.625</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G6" s="15">
         <v>44105</v>
@@ -1030,16 +1039,36 @@
       <c r="O6" s="6"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A7" s="6"/>
-      <c r="B7" s="6"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="6"/>
-      <c r="I7" s="6"/>
-      <c r="J7" s="6"/>
+      <c r="A7" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="D7" s="6">
+        <v>45</v>
+      </c>
+      <c r="E7" s="14">
+        <v>44125.916666666664</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="G7" s="14">
+        <v>44131.940972222219</v>
+      </c>
+      <c r="H7" s="15">
+        <v>44132</v>
+      </c>
+      <c r="I7" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="J7" s="6" t="s">
+        <v>34</v>
+      </c>
       <c r="K7" s="6"/>
       <c r="L7" s="6"/>
       <c r="M7" s="6"/>
@@ -1051,7 +1080,7 @@
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
       <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
+      <c r="E8" s="14"/>
       <c r="F8" s="6"/>
       <c r="G8" s="6"/>
       <c r="H8" s="6"/>
@@ -1068,7 +1097,7 @@
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
       <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
+      <c r="E9" s="14"/>
       <c r="F9" s="6"/>
       <c r="G9" s="6"/>
       <c r="H9" s="6"/>
@@ -1085,7 +1114,7 @@
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
       <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
+      <c r="E10" s="14"/>
       <c r="F10" s="6"/>
       <c r="G10" s="6"/>
       <c r="H10" s="6"/>
@@ -1102,7 +1131,7 @@
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
       <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
+      <c r="E11" s="14"/>
       <c r="F11" s="6"/>
       <c r="G11" s="6"/>
       <c r="H11" s="6"/>
@@ -1119,7 +1148,7 @@
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
       <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
+      <c r="E12" s="14"/>
       <c r="F12" s="6"/>
       <c r="G12" s="6"/>
       <c r="H12" s="6"/>
@@ -1136,7 +1165,7 @@
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
       <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
+      <c r="E13" s="14"/>
       <c r="F13" s="6"/>
       <c r="G13" s="6"/>
       <c r="H13" s="6"/>
@@ -1153,7 +1182,7 @@
       <c r="B14" s="6"/>
       <c r="C14" s="6"/>
       <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
+      <c r="E14" s="14"/>
       <c r="F14" s="6"/>
       <c r="G14" s="6"/>
       <c r="H14" s="6"/>
@@ -1170,7 +1199,7 @@
       <c r="B15" s="6"/>
       <c r="C15" s="6"/>
       <c r="D15" s="6"/>
-      <c r="E15" s="6"/>
+      <c r="E15" s="14"/>
       <c r="F15" s="6"/>
       <c r="G15" s="6"/>
       <c r="H15" s="6"/>
@@ -1187,7 +1216,7 @@
       <c r="B16" s="6"/>
       <c r="C16" s="6"/>
       <c r="D16" s="6"/>
-      <c r="E16" s="6"/>
+      <c r="E16" s="14"/>
       <c r="F16" s="6"/>
       <c r="G16" s="6"/>
       <c r="H16" s="6"/>
@@ -1204,7 +1233,7 @@
       <c r="B17" s="6"/>
       <c r="C17" s="6"/>
       <c r="D17" s="6"/>
-      <c r="E17" s="6"/>
+      <c r="E17" s="14"/>
       <c r="F17" s="6"/>
       <c r="G17" s="6"/>
       <c r="H17" s="6"/>
@@ -1221,7 +1250,7 @@
       <c r="B18" s="6"/>
       <c r="C18" s="6"/>
       <c r="D18" s="6"/>
-      <c r="E18" s="6"/>
+      <c r="E18" s="14"/>
       <c r="F18" s="6"/>
       <c r="G18" s="6"/>
       <c r="H18" s="6"/>
@@ -1238,7 +1267,7 @@
       <c r="B19" s="6"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
-      <c r="E19" s="6"/>
+      <c r="E19" s="14"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
       <c r="H19" s="6"/>
@@ -1255,7 +1284,7 @@
       <c r="B20" s="6"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
-      <c r="E20" s="6"/>
+      <c r="E20" s="14"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
       <c r="H20" s="6"/>
@@ -1825,7 +1854,7 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B2" s="17" t="s">
         <v>29</v>
@@ -1889,7 +1918,7 @@
         <v>13</v>
       </c>
       <c r="B7" s="17" t="s">
-        <v>36</v>
+        <v>54</v>
       </c>
       <c r="C7" s="6"/>
     </row>
@@ -1906,8 +1935,8 @@
       <c r="A9" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="16" t="s">
-        <v>52</v>
+      <c r="B9" s="17" t="s">
+        <v>50</v>
       </c>
       <c r="C9" s="6"/>
     </row>
@@ -1954,14 +1983,14 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="7" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B15" s="9"/>
       <c r="C15" s="6"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
-        <v>37</v>
+        <v>52</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
@@ -1975,8 +2004,16 @@
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B19" t="s">
+      <c r="B19" s="3" t="s">
         <v>53</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B20" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="C20" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
nuevos horarios rebrand AMC
</commit_message>
<xml_diff>
--- a/input.xlsx
+++ b/input.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="63">
   <si>
     <t>showFeed</t>
   </si>
@@ -169,16 +169,7 @@
     <t>lunes</t>
   </si>
   <si>
-    <t>GUARDIANES DE TRADICION</t>
-  </si>
-  <si>
     <t>MARTES</t>
-  </si>
-  <si>
-    <t>128705-NOS4A2 ON THE NEXT 205 A 206</t>
-  </si>
-  <si>
-    <t>LA VIDA OLALÁ</t>
   </si>
   <si>
     <t>MIÉRCOLES</t>
@@ -222,9 +213,6 @@
       <t>MEX adelanta la hora? 
 (Abril a Octubre)</t>
     </r>
-  </si>
-  <si>
-    <t>walking dead again and again</t>
   </si>
   <si>
     <r>
@@ -344,10 +332,37 @@
     <t>Usa el genStartDate para poner la fecha y hora de la segunda pelicula</t>
   </si>
   <si>
-    <t>QUE PEDAZO DE PELI</t>
-  </si>
-  <si>
     <t>nada</t>
+  </si>
+  <si>
+    <t>LA VIDA OLALÁ SIN BUMP</t>
+  </si>
+  <si>
+    <t>walking dead again and again con bump</t>
+  </si>
+  <si>
+    <t>walking dead again and again sin bump</t>
+  </si>
+  <si>
+    <t>GUARDIANES DE TRADICION con bump</t>
+  </si>
+  <si>
+    <t>ee</t>
+  </si>
+  <si>
+    <t>GUARDIANES DE TRADICION sin bump</t>
+  </si>
+  <si>
+    <t>mclatam</t>
+  </si>
+  <si>
+    <t>faLATAM</t>
+  </si>
+  <si>
+    <t>falatAM</t>
+  </si>
+  <si>
+    <t>fucking walking dead</t>
   </si>
 </sst>
 </file>
@@ -792,7 +807,7 @@
   <dimension ref="A1:O49"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -825,25 +840,25 @@
         <v>1</v>
       </c>
       <c r="D1" s="18" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="E1" s="12" t="s">
         <v>30</v>
       </c>
       <c r="F1" s="18" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="G1" s="18" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="H1" s="18" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="I1" s="12" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="J1" s="18" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="K1" s="11" t="s">
         <v>2</v>
@@ -863,17 +878,19 @@
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>8</v>
+        <v>39</v>
       </c>
       <c r="B2" t="s">
-        <v>40</v>
+        <v>62</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="D2" s="13"/>
+        <v>20</v>
+      </c>
+      <c r="D2" s="13">
+        <v>45</v>
+      </c>
       <c r="E2" s="14">
-        <v>44116.958333333336</v>
+        <v>44116.979166666664</v>
       </c>
       <c r="F2" s="6" t="s">
         <v>36</v>
@@ -898,13 +915,13 @@
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>42</v>
+        <v>59</v>
       </c>
       <c r="B3" t="s">
-        <v>39</v>
+        <v>53</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D3" s="13"/>
       <c r="E3" s="14">
@@ -933,13 +950,13 @@
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
-        <v>42</v>
+        <v>60</v>
       </c>
       <c r="B4" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>54</v>
+        <v>24</v>
       </c>
       <c r="D4" s="13">
         <v>60</v>
@@ -948,7 +965,7 @@
         <v>44116.958333333336</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="G4" s="15">
         <v>44116</v>
@@ -970,13 +987,13 @@
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
-        <v>8</v>
+        <v>61</v>
       </c>
       <c r="B5" t="s">
-        <v>39</v>
+        <v>55</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D5" s="13"/>
       <c r="E5" s="14">
@@ -1005,20 +1022,20 @@
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
-        <v>10</v>
+        <v>57</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>37</v>
+        <v>56</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="D6" s="13"/>
       <c r="E6" s="14">
         <v>44105.625</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G6" s="15">
         <v>44105</v>
@@ -1040,13 +1057,13 @@
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
-        <v>13</v>
+        <v>57</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D7" s="6">
         <v>45</v>
@@ -1055,7 +1072,7 @@
         <v>44125.916666666664</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="G7" s="14">
         <v>44131.940972222219</v>
@@ -1854,7 +1871,7 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B2" s="17" t="s">
         <v>29</v>
@@ -1918,7 +1935,7 @@
         <v>13</v>
       </c>
       <c r="B7" s="17" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C7" s="6"/>
     </row>
@@ -1936,7 +1953,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="17" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C9" s="6"/>
     </row>
@@ -1983,14 +2000,14 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="7" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B15" s="9"/>
       <c r="C15" s="6"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
@@ -2005,15 +2022,15 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B19" s="3" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B20" s="16" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C20" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">

</xml_diff>